<commit_message>
arregla sentido votos genlex
</commit_message>
<xml_diff>
--- a/clases/13peliSuiza/votaciones-nominales/proces-verbal-3-votes.xlsx
+++ b/clases/13peliSuiza/votaciones-nominales/proces-verbal-3-votes.xlsx
@@ -802,31 +802,31 @@
     <t xml:space="preserve">Résultat du 1er vote (Heberlein+Baader ou Imhof)</t>
   </si>
   <si>
+    <t xml:space="preserve">Proposition de la majorité 5 ans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposition de la majorité (ou Minorité II)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sentido =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposition Imhof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposition de la minorité I (Kunz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposition Baader (ou Imhof)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résultat du 2e vote (Majorité ou Minorité Kunz)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Proposition de la minorité II (Graf) 10 ans</t>
   </si>
   <si>
     <t xml:space="preserve">Proposition de la minorité III (Randegger) sans moratoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sentido =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposition Imhof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposition de la minorité I (Kunz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposition Baader (ou Imhof)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résultat du 2e vote (Majorité ou Minorité Kunz)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposition de la majorité 5 ans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proposition de la majorité (ou Minorité II)</t>
   </si>
   <si>
     <t xml:space="preserve">+ ja / oui / sì</t>
@@ -960,15 +960,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -980,21 +971,22 @@
   <dimension ref="A1:O215"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E188" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E197" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A188" activeCellId="0" sqref="A188"/>
-      <selection pane="bottomRight" activeCell="C203" activeCellId="0" sqref="C203"/>
+      <selection pane="bottomLeft" activeCell="A197" activeCellId="0" sqref="A197"/>
+      <selection pane="bottomRight" activeCell="E204" activeCellId="0" sqref="E204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="17.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="2.31"/>
   </cols>
   <sheetData>
@@ -9920,7 +9912,7 @@
         <v>260</v>
       </c>
       <c r="O204" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9958,7 +9950,7 @@
         <v>267</v>
       </c>
       <c r="O205" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>